<commit_message>
updated excel file layout
</commit_message>
<xml_diff>
--- a/resultat.xlsx
+++ b/resultat.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msldk\Desktop\Uni\SoftwareTeknologi\2Semester\GFV\Journal4_gruppe42\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msldk\Desktop\Uni\SoftwareTeknologi\2Semester\GFV\Journal4_gruppe42\GFV_LocalRepo\GFVJournal4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E8B86D-D122-49F9-BCCF-2FA9542722D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A380F10D-9B57-4863-80AA-17FBF1D0229D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14160" xr2:uid="{FAFF625E-B176-4C97-9976-A2D0AF4F6A25}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
   <si>
     <t>Vægt g</t>
   </si>
@@ -77,12 +77,27 @@
   <si>
     <t xml:space="preserve">EFTER 1 time </t>
   </si>
+  <si>
+    <t>Efter ca 2 timers tid</t>
+  </si>
+  <si>
+    <t>FIND LINÆRT OMRÅDE</t>
+  </si>
+  <si>
+    <t>LINÆR REGRESSION FIND HÆLDNING</t>
+  </si>
+  <si>
+    <t>FIND PRÆCISION INDEN FOR 95% FAXEKONDI</t>
+  </si>
+  <si>
+    <t>EFTER 2 TIMER CA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,8 +113,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,6 +131,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -125,12 +153,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -149,553 +179,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>ADC value vs vægt ref (204</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> g preloaded)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Result!$D$15</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Vægt ref g</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-DK"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Result!$B$16:$B$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>336</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>515</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>699</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>880</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1060</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1244</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1425</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1608</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1790</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1974</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Result!$D$16:$D$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>900</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-14BF-4974-B486-4DB1870C1693}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2037806127"/>
-        <c:axId val="2037805295"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="2037806127"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>ADC Value </a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2037805295"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="2037805295"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>reference</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> vægt [g]</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2037806127"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-DK"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -780,7 +263,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Result!$C$1</c:f>
+              <c:f>Result!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -863,7 +346,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Result!$B$2:$B$12</c:f>
+              <c:f>Result!$B$3:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -905,7 +388,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Result!$C$2:$C$12</c:f>
+              <c:f>Result!$C$3:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -948,7 +431,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-62A6-45BE-B53F-719242AE2F19}"/>
+              <c16:uniqueId val="{00000001-B880-4F39-A975-0245FCCC8721}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1257,6 +740,1154 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ADC value vs vægt ref (204</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> g preloaded)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Result!$D$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vægt ref g</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-DK"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Result!$B$26:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1244</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1425</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1608</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1790</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1974</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Result!$D$26:$D$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1C10-4673-8528-6727AEF593BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2037806127"/>
+        <c:axId val="2037805295"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2037806127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>ADC Value </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2037805295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2037805295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>reference</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> vægt [g]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2037806127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ADC value vs vægt ref (204</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> g preloaded) efter 2 timer ca</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Result!$J$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vægt ref g</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.16723061290663177"/>
+                  <c:y val="-3.9058084183625635E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Result!$H$26:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>879</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1233</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1607</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1790</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1954</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Result!$J$26:$J$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0292-4FE9-A8FE-041E4FA0B435}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2037806127"/>
+        <c:axId val="2037805295"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Result!$D$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Vægt ref g</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:trendline>
+                  <c:spPr>
+                    <a:ln w="19050" cap="rnd">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:prstDash val="sysDot"/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:trendlineType val="linear"/>
+                  <c:dispRSqr val="1"/>
+                  <c:dispEq val="1"/>
+                  <c:trendlineLbl>
+                    <c:numFmt formatCode="General" sourceLinked="0"/>
+                    <c:spPr>
+                      <a:noFill/>
+                      <a:ln>
+                        <a:noFill/>
+                      </a:ln>
+                      <a:effectLst/>
+                    </c:spPr>
+                    <c:txPr>
+                      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                      <a:lstStyle/>
+                      <a:p>
+                        <a:pPr>
+                          <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="65000"/>
+                                <a:lumOff val="35000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:defRPr>
+                        </a:pPr>
+                        <a:endParaRPr lang="en-DK"/>
+                      </a:p>
+                    </c:txPr>
+                  </c:trendlineLbl>
+                </c:trendline>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Result!$B$26:$B$35</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>336</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>515</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>699</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>880</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1060</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1244</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1425</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1608</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1790</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>1974</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Result!$D$26:$D$35</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>400</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>500</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>600</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>700</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>800</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>900</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-0292-4FE9-A8FE-041E4FA0B435}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2037806127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>ADC Value </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2037805295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2037805295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>reference</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> vægt [g]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2037806127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2373,23 +3004,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>606484</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>107324</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Diagram 4">
+        <xdr:cNvPr id="8" name="Diagram 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2EE1FCB-8C44-4434-A0F6-FADF1F90B572}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FB51A68-9A4E-4C76-AB08-B58E79A8DBE6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2411,23 +3042,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>591226</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3068</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>160987</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Diagram 2">
+        <xdr:cNvPr id="13" name="Diagram 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BC6A962-157A-47A2-B8B9-612453F57059}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4197C239-700B-4DF3-9255-5953248FC6E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2442,6 +3073,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>660551</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>151126</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{790B2D20-F605-4D9B-80FD-10B5AA0AB8F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2747,10 +3416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903540F4-C1F6-4C83-A85B-132A43DBB526}">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScale="104" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2761,62 +3430,53 @@
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <f>B2-$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>292</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A12" si="0">B3-$B$2</f>
-        <v>1</v>
+        <f>B3-$B$3</f>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C3" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <f t="shared" si="0"/>
-        <v>37</v>
+        <f t="shared" ref="A4:A13" si="0">B4-$B$3</f>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>329</v>
+        <v>293</v>
       </c>
       <c r="C4" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -2824,13 +3484,13 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
-        <v>215</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1">
-        <v>507</v>
+        <v>329</v>
       </c>
       <c r="C5" s="1">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2838,13 +3498,13 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
-        <v>395</v>
+        <v>215</v>
       </c>
       <c r="B6" s="1">
-        <v>687</v>
+        <v>507</v>
       </c>
       <c r="C6" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2852,13 +3512,13 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
-        <v>577</v>
+        <v>395</v>
       </c>
       <c r="B7" s="1">
-        <v>869</v>
+        <v>687</v>
       </c>
       <c r="C7" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -2866,13 +3526,13 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
-        <v>762</v>
+        <v>577</v>
       </c>
       <c r="B8" s="1">
-        <v>1054</v>
+        <v>869</v>
       </c>
       <c r="C8" s="1">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2880,13 +3540,13 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
-        <v>943</v>
+        <v>762</v>
       </c>
       <c r="B9" s="1">
-        <v>1235</v>
+        <v>1054</v>
       </c>
       <c r="C9" s="1">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -2894,13 +3554,13 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
-        <v>1123</v>
+        <v>943</v>
       </c>
       <c r="B10" s="1">
-        <v>1415</v>
+        <v>1235</v>
       </c>
       <c r="C10" s="1">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -2908,13 +3568,13 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
-        <v>1218</v>
+        <v>1123</v>
       </c>
       <c r="B11" s="1">
-        <v>1510</v>
+        <v>1415</v>
       </c>
       <c r="C11" s="1">
-        <v>850</v>
+        <v>800</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2922,795 +3582,611 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
-        <v>1310</v>
+        <v>1218</v>
       </c>
       <c r="B12" s="1">
-        <v>1602</v>
+        <v>1510</v>
       </c>
       <c r="C12" s="1">
-        <v>900</v>
+        <v>850</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>1310</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1602</v>
+      </c>
+      <c r="C13" s="1">
+        <v>900</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="G24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B16">
+      <c r="E25" s="2"/>
+      <c r="G25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B26">
         <v>336</v>
       </c>
-      <c r="C16" s="3">
-        <f>(B16*$A$27)-184</f>
+      <c r="C26" s="3">
+        <f t="shared" ref="C26:C35" si="1">(B26*$A$37)-184</f>
         <v>0.46400000000002706</v>
       </c>
-      <c r="D16">
+      <c r="D26">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B17">
+      <c r="H26">
+        <v>333</v>
+      </c>
+      <c r="I26" s="3">
+        <f>(H26*$A$37)-183</f>
+        <v>-0.18299999999999272</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B27">
         <v>515</v>
       </c>
-      <c r="C17" s="3">
-        <f>(B17*$A$27)-184</f>
+      <c r="C27" s="3">
+        <f t="shared" si="1"/>
         <v>98.735000000000014</v>
       </c>
-      <c r="D17">
+      <c r="D27">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B18">
+      <c r="H27">
+        <v>512</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" ref="I27:I35" si="2">(H27*$A$37)-183</f>
+        <v>98.088000000000022</v>
+      </c>
+      <c r="J27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B28">
         <v>699</v>
       </c>
-      <c r="C18" s="3">
-        <f>(B18*$A$27)-184</f>
+      <c r="C28" s="3">
+        <f t="shared" si="1"/>
         <v>199.75100000000003</v>
       </c>
-      <c r="D18">
+      <c r="D28">
         <v>200</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B19">
+      <c r="H28">
+        <v>701</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="2"/>
+        <v>201.84900000000005</v>
+      </c>
+      <c r="J28">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B29">
         <v>880</v>
       </c>
-      <c r="C19" s="3">
-        <f>(B19*$A$27)-184</f>
+      <c r="C29" s="3">
+        <f t="shared" si="1"/>
         <v>299.12000000000006</v>
       </c>
-      <c r="D19">
+      <c r="D29">
         <v>300</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B20">
+      <c r="H29">
+        <v>879</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="2"/>
+        <v>299.57100000000003</v>
+      </c>
+      <c r="J29">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B30">
         <v>1060</v>
       </c>
-      <c r="C20" s="3">
-        <f>(B20*$A$27)-184</f>
+      <c r="C30" s="3">
+        <f t="shared" si="1"/>
         <v>397.94000000000005</v>
       </c>
-      <c r="D20">
+      <c r="D30">
         <v>400</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B21">
+      <c r="H30">
+        <v>1050</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="2"/>
+        <v>393.45000000000005</v>
+      </c>
+      <c r="J30">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B31">
         <v>1244</v>
       </c>
-      <c r="C21" s="3">
-        <f>(B21*$A$27)-184</f>
+      <c r="C31" s="3">
+        <f t="shared" si="1"/>
         <v>498.95600000000002</v>
       </c>
-      <c r="D21">
+      <c r="D31">
         <v>500</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B22">
+      <c r="H31">
+        <v>1233</v>
+      </c>
+      <c r="I31" s="3">
+        <f t="shared" si="2"/>
+        <v>493.91700000000003</v>
+      </c>
+      <c r="J31">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B32">
         <v>1425</v>
       </c>
-      <c r="C22" s="3">
-        <f>(B22*$A$27)-184</f>
+      <c r="C32" s="3">
+        <f t="shared" si="1"/>
         <v>598.32500000000005</v>
       </c>
-      <c r="D22">
+      <c r="D32">
         <v>600</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B23">
+      <c r="H32">
+        <v>1450</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="2"/>
+        <v>613.05000000000007</v>
+      </c>
+      <c r="J32">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B33">
         <v>1608</v>
       </c>
-      <c r="C23" s="3">
-        <f>(B23*$A$27)-184</f>
+      <c r="C33" s="3">
+        <f t="shared" si="1"/>
         <v>698.79200000000003</v>
       </c>
-      <c r="D23">
+      <c r="D33">
         <v>700</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B24">
+      <c r="H33">
+        <v>1607</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="2"/>
+        <v>699.24300000000005</v>
+      </c>
+      <c r="J33">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B34">
         <v>1790</v>
       </c>
-      <c r="C24" s="3">
-        <f>(B24*$A$27)-184</f>
+      <c r="C34" s="3">
+        <f t="shared" si="1"/>
         <v>798.71</v>
       </c>
-      <c r="D24">
+      <c r="D34">
         <v>800</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B25">
+      <c r="H34">
+        <v>1790</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="2"/>
+        <v>799.71</v>
+      </c>
+      <c r="J34">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B35">
         <v>1974</v>
       </c>
-      <c r="C25" s="3">
-        <f>(B25*$A$27)-184</f>
+      <c r="C35" s="3">
+        <f t="shared" si="1"/>
         <v>899.72600000000011</v>
       </c>
-      <c r="D25">
+      <c r="D35">
         <v>900</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="H35">
+        <v>1954</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="2"/>
+        <v>889.74600000000009</v>
+      </c>
+      <c r="J35">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27">
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37">
         <v>0.54900000000000004</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="G37">
+        <v>0.55049999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A52" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>10</v>
       </c>
-      <c r="B31">
+      <c r="B54">
         <v>10</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D54" t="s">
         <v>10</v>
       </c>
-      <c r="E31">
+      <c r="E54">
         <v>10</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G54" t="s">
         <v>10</v>
       </c>
-      <c r="H31">
+      <c r="H54">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>7</v>
       </c>
-      <c r="B32">
-        <f>SUM(A38:A47)/B31</f>
+      <c r="B55">
+        <f>SUM(A61:A70)/B54</f>
         <v>204.5</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D55" t="s">
         <v>7</v>
       </c>
-      <c r="E32">
-        <f>SUM(D38:D47)/E31</f>
+      <c r="E55">
+        <f>SUM(D61:D70)/E54</f>
         <v>499.4</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G55" t="s">
         <v>7</v>
       </c>
-      <c r="H32">
-        <f>SUM(G38:G47)/H31</f>
+      <c r="H55">
+        <f>SUM(G61:G70)/H54</f>
         <v>704.8</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>8</v>
       </c>
-      <c r="B33">
-        <f>B32/B31-1</f>
+      <c r="B56">
+        <f>B55/B54-1</f>
         <v>19.45</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D56" t="s">
         <v>8</v>
       </c>
-      <c r="E33">
-        <f>E32/E31-1</f>
+      <c r="E56">
+        <f>E55/E54-1</f>
         <v>48.94</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G56" t="s">
         <v>8</v>
       </c>
-      <c r="H33">
-        <f>H32/H31-1</f>
+      <c r="H56">
+        <f>H55/H54-1</f>
         <v>69.47999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>9</v>
       </c>
-      <c r="B34">
-        <f>SQRT(B33)</f>
+      <c r="B57">
+        <f>SQRT(B56)</f>
         <v>4.410215414239989</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D57" t="s">
         <v>9</v>
       </c>
-      <c r="E34">
-        <f>SQRT(E33)</f>
+      <c r="E57">
+        <f>SQRT(E56)</f>
         <v>6.9957129729570804</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G57" t="s">
         <v>9</v>
       </c>
-      <c r="H34">
-        <f>SQRT(H33)</f>
+      <c r="H57">
+        <f>SQRT(H56)</f>
         <v>8.3354663936698827</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>11</v>
       </c>
-      <c r="B35">
-        <f>B34*1.96</f>
+      <c r="B58">
+        <f>B57*1.96</f>
         <v>8.6440222119103787</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D58" t="s">
         <v>11</v>
       </c>
-      <c r="E35">
-        <f>E34*1.96</f>
+      <c r="E58">
+        <f>E57*1.96</f>
         <v>13.711597426995878</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G58" t="s">
         <v>11</v>
       </c>
-      <c r="H35">
-        <f>H34*1.96</f>
+      <c r="H58">
+        <f>H57*1.96</f>
         <v>16.337514131592968</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="4" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A60" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4" t="s">
+      <c r="C60" s="4"/>
+      <c r="D60" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E60" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4" t="s">
+      <c r="F60" s="4"/>
+      <c r="G60" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="H60" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A61">
         <v>205</v>
-      </c>
-      <c r="B38">
-        <v>201</v>
-      </c>
-      <c r="D38">
-        <v>498</v>
-      </c>
-      <c r="E38">
-        <v>500</v>
-      </c>
-      <c r="G38">
-        <v>702</v>
-      </c>
-      <c r="H38">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>204</v>
-      </c>
-      <c r="B39">
-        <v>201</v>
-      </c>
-      <c r="D39">
-        <v>500</v>
-      </c>
-      <c r="E39">
-        <v>500</v>
-      </c>
-      <c r="G39">
-        <v>708</v>
-      </c>
-      <c r="H39">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>204</v>
-      </c>
-      <c r="B40">
-        <v>201</v>
-      </c>
-      <c r="D40">
-        <v>499</v>
-      </c>
-      <c r="E40">
-        <v>500</v>
-      </c>
-      <c r="G40">
-        <v>704</v>
-      </c>
-      <c r="H40">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <v>205</v>
-      </c>
-      <c r="B41">
-        <v>201</v>
-      </c>
-      <c r="D41">
-        <v>498</v>
-      </c>
-      <c r="E41">
-        <v>500</v>
-      </c>
-      <c r="G41">
-        <v>705</v>
-      </c>
-      <c r="H41">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <v>204</v>
-      </c>
-      <c r="B42">
-        <v>201</v>
-      </c>
-      <c r="D42">
-        <v>500</v>
-      </c>
-      <c r="E42">
-        <v>500</v>
-      </c>
-      <c r="G42">
-        <v>705</v>
-      </c>
-      <c r="H42">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>205</v>
-      </c>
-      <c r="B43">
-        <v>201</v>
-      </c>
-      <c r="D43">
-        <v>499</v>
-      </c>
-      <c r="E43">
-        <v>500</v>
-      </c>
-      <c r="G43">
-        <v>706</v>
-      </c>
-      <c r="H43">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <v>204</v>
-      </c>
-      <c r="B44">
-        <v>201</v>
-      </c>
-      <c r="D44">
-        <v>500</v>
-      </c>
-      <c r="E44">
-        <v>500</v>
-      </c>
-      <c r="G44">
-        <v>705</v>
-      </c>
-      <c r="H44">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>205</v>
-      </c>
-      <c r="B45">
-        <v>201</v>
-      </c>
-      <c r="D45">
-        <v>500</v>
-      </c>
-      <c r="E45">
-        <v>500</v>
-      </c>
-      <c r="G45">
-        <v>705</v>
-      </c>
-      <c r="H45">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <v>204</v>
-      </c>
-      <c r="B46">
-        <v>201</v>
-      </c>
-      <c r="D46">
-        <v>500</v>
-      </c>
-      <c r="E46">
-        <v>500</v>
-      </c>
-      <c r="G46">
-        <v>704</v>
-      </c>
-      <c r="H46">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47">
-        <v>205</v>
-      </c>
-      <c r="B47">
-        <v>201</v>
-      </c>
-      <c r="D47">
-        <v>500</v>
-      </c>
-      <c r="E47">
-        <v>500</v>
-      </c>
-      <c r="G47">
-        <v>704</v>
-      </c>
-      <c r="H47">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50">
-        <v>10</v>
-      </c>
-      <c r="D50" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50">
-        <v>10</v>
-      </c>
-      <c r="G50" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>7</v>
-      </c>
-      <c r="B51">
-        <f>SUM(A57:A66)/B50</f>
-        <v>194.3</v>
-      </c>
-      <c r="D51" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51">
-        <f>SUM(D57:D66)/E50</f>
-        <v>494.8</v>
-      </c>
-      <c r="G51" t="s">
-        <v>7</v>
-      </c>
-      <c r="H51">
-        <f>SUM(G57:G66)/H50</f>
-        <v>697</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52">
-        <f>B51/B50-1</f>
-        <v>18.43</v>
-      </c>
-      <c r="D52" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52">
-        <f>E51/E50-1</f>
-        <v>48.480000000000004</v>
-      </c>
-      <c r="G52" t="s">
-        <v>8</v>
-      </c>
-      <c r="H52">
-        <f>H51/H50-1</f>
-        <v>68.7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>9</v>
-      </c>
-      <c r="B53">
-        <f>SQRT(B52)</f>
-        <v>4.2930175867331357</v>
-      </c>
-      <c r="D53" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53">
-        <f>SQRT(E52)</f>
-        <v>6.9627580742116848</v>
-      </c>
-      <c r="G53" t="s">
-        <v>9</v>
-      </c>
-      <c r="H53">
-        <f>SQRT(H52)</f>
-        <v>8.2885463140408397</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>11</v>
-      </c>
-      <c r="B54">
-        <f>B53*1.96</f>
-        <v>8.4143144699969454</v>
-      </c>
-      <c r="D54" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54">
-        <f>E53*1.96</f>
-        <v>13.647005825454903</v>
-      </c>
-      <c r="G54" t="s">
-        <v>11</v>
-      </c>
-      <c r="H54">
-        <f>H53*1.96</f>
-        <v>16.245550775520044</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A56" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A57">
-        <v>197</v>
-      </c>
-      <c r="B57">
-        <v>201</v>
-      </c>
-      <c r="D57">
-        <v>494</v>
-      </c>
-      <c r="E57">
-        <v>500</v>
-      </c>
-      <c r="G57">
-        <v>695</v>
-      </c>
-      <c r="H57">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A58">
-        <v>195</v>
-      </c>
-      <c r="B58">
-        <v>201</v>
-      </c>
-      <c r="D58">
-        <v>495</v>
-      </c>
-      <c r="E58">
-        <v>500</v>
-      </c>
-      <c r="G58">
-        <v>698</v>
-      </c>
-      <c r="H58">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <v>194</v>
-      </c>
-      <c r="B59">
-        <v>201</v>
-      </c>
-      <c r="D59">
-        <v>494</v>
-      </c>
-      <c r="E59">
-        <v>500</v>
-      </c>
-      <c r="G59">
-        <v>697</v>
-      </c>
-      <c r="H59">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <v>192</v>
-      </c>
-      <c r="B60">
-        <v>201</v>
-      </c>
-      <c r="D60">
-        <v>496</v>
-      </c>
-      <c r="E60">
-        <v>500</v>
-      </c>
-      <c r="G60">
-        <v>697</v>
-      </c>
-      <c r="H60">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>194</v>
       </c>
       <c r="B61">
         <v>201</v>
       </c>
       <c r="D61">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="E61">
         <v>500</v>
       </c>
       <c r="G61">
-        <v>697</v>
+        <v>702</v>
       </c>
       <c r="H61">
         <v>703</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="B62">
         <v>201</v>
       </c>
       <c r="D62">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="E62">
         <v>500</v>
       </c>
       <c r="G62">
-        <v>697</v>
+        <v>708</v>
       </c>
       <c r="H62">
         <v>703</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="B63">
         <v>201</v>
       </c>
       <c r="D63">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="E63">
         <v>500</v>
       </c>
       <c r="G63">
-        <v>698</v>
+        <v>704</v>
       </c>
       <c r="H63">
         <v>703</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="B64">
         <v>201</v>
       </c>
       <c r="D64">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="E64">
         <v>500</v>
       </c>
       <c r="G64">
-        <v>697</v>
+        <v>705</v>
       </c>
       <c r="H64">
         <v>703</v>
@@ -3718,19 +4194,19 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="B65">
         <v>201</v>
       </c>
       <c r="D65">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="E65">
         <v>500</v>
       </c>
       <c r="G65">
-        <v>697</v>
+        <v>705</v>
       </c>
       <c r="H65">
         <v>703</v>
@@ -3738,21 +4214,440 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="B66">
         <v>201</v>
       </c>
       <c r="D66">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="E66">
         <v>500</v>
       </c>
       <c r="G66">
+        <v>706</v>
+      </c>
+      <c r="H66">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>204</v>
+      </c>
+      <c r="B67">
+        <v>201</v>
+      </c>
+      <c r="D67">
+        <v>500</v>
+      </c>
+      <c r="E67">
+        <v>500</v>
+      </c>
+      <c r="G67">
+        <v>705</v>
+      </c>
+      <c r="H67">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>205</v>
+      </c>
+      <c r="B68">
+        <v>201</v>
+      </c>
+      <c r="D68">
+        <v>500</v>
+      </c>
+      <c r="E68">
+        <v>500</v>
+      </c>
+      <c r="G68">
+        <v>705</v>
+      </c>
+      <c r="H68">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>204</v>
+      </c>
+      <c r="B69">
+        <v>201</v>
+      </c>
+      <c r="D69">
+        <v>500</v>
+      </c>
+      <c r="E69">
+        <v>500</v>
+      </c>
+      <c r="G69">
+        <v>704</v>
+      </c>
+      <c r="H69">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>205</v>
+      </c>
+      <c r="B70">
+        <v>201</v>
+      </c>
+      <c r="D70">
+        <v>500</v>
+      </c>
+      <c r="E70">
+        <v>500</v>
+      </c>
+      <c r="G70">
+        <v>704</v>
+      </c>
+      <c r="H70">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73">
+        <v>10</v>
+      </c>
+      <c r="D73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73">
+        <v>10</v>
+      </c>
+      <c r="G73" t="s">
+        <v>10</v>
+      </c>
+      <c r="H73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74">
+        <f>SUM(A80:A89)/B73</f>
+        <v>194.3</v>
+      </c>
+      <c r="D74" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74">
+        <f>SUM(D80:D89)/E73</f>
+        <v>494.8</v>
+      </c>
+      <c r="G74" t="s">
+        <v>7</v>
+      </c>
+      <c r="H74">
+        <f>SUM(G80:G89)/H73</f>
         <v>697</v>
       </c>
-      <c r="H66">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75">
+        <f>B74/B73-1</f>
+        <v>18.43</v>
+      </c>
+      <c r="D75" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75">
+        <f>E74/E73-1</f>
+        <v>48.480000000000004</v>
+      </c>
+      <c r="G75" t="s">
+        <v>8</v>
+      </c>
+      <c r="H75">
+        <f>H74/H73-1</f>
+        <v>68.7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76">
+        <f>SQRT(B75)</f>
+        <v>4.2930175867331357</v>
+      </c>
+      <c r="D76" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76">
+        <f>SQRT(E75)</f>
+        <v>6.9627580742116848</v>
+      </c>
+      <c r="G76" t="s">
+        <v>9</v>
+      </c>
+      <c r="H76">
+        <f>SQRT(H75)</f>
+        <v>8.2885463140408397</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>11</v>
+      </c>
+      <c r="B77">
+        <f>B76*1.96</f>
+        <v>8.4143144699969454</v>
+      </c>
+      <c r="D77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77">
+        <f>E76*1.96</f>
+        <v>13.647005825454903</v>
+      </c>
+      <c r="G77" t="s">
+        <v>11</v>
+      </c>
+      <c r="H77">
+        <f>H76*1.96</f>
+        <v>16.245550775520044</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>197</v>
+      </c>
+      <c r="B80">
+        <v>201</v>
+      </c>
+      <c r="D80">
+        <v>494</v>
+      </c>
+      <c r="E80">
+        <v>500</v>
+      </c>
+      <c r="G80">
+        <v>695</v>
+      </c>
+      <c r="H80">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>195</v>
+      </c>
+      <c r="B81">
+        <v>201</v>
+      </c>
+      <c r="D81">
+        <v>495</v>
+      </c>
+      <c r="E81">
+        <v>500</v>
+      </c>
+      <c r="G81">
+        <v>698</v>
+      </c>
+      <c r="H81">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>194</v>
+      </c>
+      <c r="B82">
+        <v>201</v>
+      </c>
+      <c r="D82">
+        <v>494</v>
+      </c>
+      <c r="E82">
+        <v>500</v>
+      </c>
+      <c r="G82">
+        <v>697</v>
+      </c>
+      <c r="H82">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>192</v>
+      </c>
+      <c r="B83">
+        <v>201</v>
+      </c>
+      <c r="D83">
+        <v>496</v>
+      </c>
+      <c r="E83">
+        <v>500</v>
+      </c>
+      <c r="G83">
+        <v>697</v>
+      </c>
+      <c r="H83">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>194</v>
+      </c>
+      <c r="B84">
+        <v>201</v>
+      </c>
+      <c r="D84">
+        <v>495</v>
+      </c>
+      <c r="E84">
+        <v>500</v>
+      </c>
+      <c r="G84">
+        <v>697</v>
+      </c>
+      <c r="H84">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>195</v>
+      </c>
+      <c r="B85">
+        <v>201</v>
+      </c>
+      <c r="D85">
+        <v>495</v>
+      </c>
+      <c r="E85">
+        <v>500</v>
+      </c>
+      <c r="G85">
+        <v>697</v>
+      </c>
+      <c r="H85">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>194</v>
+      </c>
+      <c r="B86">
+        <v>201</v>
+      </c>
+      <c r="D86">
+        <v>494</v>
+      </c>
+      <c r="E86">
+        <v>500</v>
+      </c>
+      <c r="G86">
+        <v>698</v>
+      </c>
+      <c r="H86">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>194</v>
+      </c>
+      <c r="B87">
+        <v>201</v>
+      </c>
+      <c r="D87">
+        <v>495</v>
+      </c>
+      <c r="E87">
+        <v>500</v>
+      </c>
+      <c r="G87">
+        <v>697</v>
+      </c>
+      <c r="H87">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>195</v>
+      </c>
+      <c r="B88">
+        <v>201</v>
+      </c>
+      <c r="D88">
+        <v>496</v>
+      </c>
+      <c r="E88">
+        <v>500</v>
+      </c>
+      <c r="G88">
+        <v>697</v>
+      </c>
+      <c r="H88">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>193</v>
+      </c>
+      <c r="B89">
+        <v>201</v>
+      </c>
+      <c r="D89">
+        <v>494</v>
+      </c>
+      <c r="E89">
+        <v>500</v>
+      </c>
+      <c r="G89">
+        <v>697</v>
+      </c>
+      <c r="H89">
         <v>703</v>
       </c>
     </row>

</xml_diff>